<commit_message>
valuation of kalimasta, sattidanand bhawan, and estimate of khulaltaar dhikurepaati
</commit_message>
<xml_diff>
--- a/ofc/estimates/Finalized valuations/kalimasta mandir/valuation kalimasta.xlsx
+++ b/ofc/estimates/Finalized valuations/kalimasta mandir/valuation kalimasta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="kalimasta mandir final" sheetId="17" state="hidden" r:id="rId1"/>
@@ -716,6 +716,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -732,31 +742,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -784,6 +769,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1424,113 +1424,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
     </row>
     <row r="5" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
     </row>
     <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -2615,11 +2615,11 @@
       <c r="B47" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="73">
+      <c r="C47" s="67">
         <f>J45</f>
         <v>345993.93824887183</v>
       </c>
-      <c r="D47" s="73"/>
+      <c r="D47" s="67"/>
       <c r="E47" s="40">
         <v>100</v>
       </c>
@@ -2635,10 +2635,10 @@
       <c r="B48" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="76">
+      <c r="C48" s="70">
         <v>300000</v>
       </c>
-      <c r="D48" s="76"/>
+      <c r="D48" s="70"/>
       <c r="E48" s="40"/>
       <c r="F48" s="46"/>
       <c r="G48" s="45"/>
@@ -2652,11 +2652,11 @@
       <c r="B49" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="76">
+      <c r="C49" s="70">
         <f>C48-C51-C52</f>
         <v>285000</v>
       </c>
-      <c r="D49" s="76"/>
+      <c r="D49" s="70"/>
       <c r="E49" s="40">
         <f>C49/C47*100</f>
         <v>82.371385302999386</v>
@@ -2673,11 +2673,11 @@
       <c r="B50" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="73">
+      <c r="C50" s="67">
         <f>C47-C49</f>
         <v>60993.938248871826</v>
       </c>
-      <c r="D50" s="73"/>
+      <c r="D50" s="67"/>
       <c r="E50" s="40">
         <f>100-E49</f>
         <v>17.628614697000614</v>
@@ -2694,11 +2694,11 @@
       <c r="B51" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="73">
+      <c r="C51" s="67">
         <f>C48*0.03</f>
         <v>9000</v>
       </c>
-      <c r="D51" s="73"/>
+      <c r="D51" s="67"/>
       <c r="E51" s="40">
         <v>3</v>
       </c>
@@ -2714,11 +2714,11 @@
       <c r="B52" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="73">
+      <c r="C52" s="67">
         <f>C48*0.02</f>
         <v>6000</v>
       </c>
-      <c r="D52" s="73"/>
+      <c r="D52" s="67"/>
       <c r="E52" s="40">
         <v>2</v>
       </c>
@@ -2800,6 +2800,13 @@
     <row r="109" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="A7:F7"/>
@@ -2808,13 +2815,6 @@
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2831,7 +2831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -2851,113 +2851,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
     </row>
     <row r="5" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
     </row>
     <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -4199,11 +4199,11 @@
       <c r="B50" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="73">
+      <c r="C50" s="67">
         <f>J48</f>
         <v>344235.93318674725</v>
       </c>
-      <c r="D50" s="73"/>
+      <c r="D50" s="67"/>
       <c r="E50" s="40">
         <v>100</v>
       </c>
@@ -4219,10 +4219,10 @@
       <c r="B51" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="76">
+      <c r="C51" s="70">
         <v>300000</v>
       </c>
-      <c r="D51" s="76"/>
+      <c r="D51" s="70"/>
       <c r="E51" s="40"/>
       <c r="F51" s="46"/>
       <c r="G51" s="45"/>
@@ -4236,11 +4236,11 @@
       <c r="B52" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="76">
+      <c r="C52" s="70">
         <f>C51-C54-C55</f>
         <v>285000</v>
       </c>
-      <c r="D52" s="76"/>
+      <c r="D52" s="70"/>
       <c r="E52" s="40">
         <f>C52/C50*100</f>
         <v>82.792054089654883</v>
@@ -4257,11 +4257,11 @@
       <c r="B53" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="73">
+      <c r="C53" s="67">
         <f>C50-C52</f>
         <v>59235.93318674725</v>
       </c>
-      <c r="D53" s="73"/>
+      <c r="D53" s="67"/>
       <c r="E53" s="40">
         <f>100-E52</f>
         <v>17.207945910345117</v>
@@ -4278,11 +4278,11 @@
       <c r="B54" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C54" s="73">
+      <c r="C54" s="67">
         <f>C51*0.03</f>
         <v>9000</v>
       </c>
-      <c r="D54" s="73"/>
+      <c r="D54" s="67"/>
       <c r="E54" s="40">
         <v>3</v>
       </c>
@@ -4298,11 +4298,11 @@
       <c r="B55" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C55" s="73">
+      <c r="C55" s="67">
         <f>C51*0.02</f>
         <v>6000</v>
       </c>
-      <c r="D55" s="73"/>
+      <c r="D55" s="67"/>
       <c r="E55" s="40">
         <v>2</v>
       </c>
@@ -4384,13 +4384,6 @@
     <row r="112" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="A7:F7"/>
@@ -4399,6 +4392,13 @@
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -4415,7 +4415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -4435,90 +4435,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
     </row>
     <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
     </row>
     <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="77">
+      <c r="C6" s="86">
         <f>F24</f>
         <v>344235.93318674725</v>
       </c>
-      <c r="D6" s="78"/>
+      <c r="D6" s="87"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -4526,11 +4526,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="77">
+      <c r="J6" s="86">
         <f>I24</f>
         <v>351068.54966387467</v>
       </c>
-      <c r="K6" s="78"/>
+      <c r="K6" s="87"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -4539,77 +4539,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="I7" s="85" t="s">
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="I7" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="67" t="str">
+      <c r="A8" s="71" t="str">
         <f>'kalimasta mandir final (2)'!A6:F6</f>
         <v>Project:- कालीमस्ट मन्दिर निर्माण</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="I8" s="86" t="s">
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="I8" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="J8" s="86"/>
-      <c r="K8" s="86"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="87" t="str">
+      <c r="A9" s="82" t="str">
         <f>'kalimasta mandir final (2)'!A7:F7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="I9" s="86" t="s">
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="I9" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="82" t="s">
+      <c r="C11" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="90" t="s">
+      <c r="D11" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90" t="s">
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="82" t="s">
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="83" t="s">
+      <c r="K11" s="78" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="82"/>
-      <c r="B12" s="89"/>
-      <c r="C12" s="82"/>
+      <c r="A12" s="77"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="77"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -4628,8 +4628,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="82"/>
-      <c r="K12" s="83"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="78"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
@@ -4956,6 +4956,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -4969,16 +4976,9 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;LPrepared By:
@@ -4993,7 +4993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
@@ -5016,113 +5016,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
     </row>
     <row r="5" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="76" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
     </row>
     <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="68" t="s">
+      <c r="H6" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -6731,11 +6731,11 @@
       <c r="B57" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C57" s="73">
+      <c r="C57" s="67">
         <f>J55</f>
         <v>351068.54966387467</v>
       </c>
-      <c r="D57" s="73"/>
+      <c r="D57" s="67"/>
       <c r="E57" s="40">
         <v>100</v>
       </c>
@@ -6751,10 +6751,10 @@
       <c r="B58" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C58" s="76">
+      <c r="C58" s="70">
         <v>300000</v>
       </c>
-      <c r="D58" s="76"/>
+      <c r="D58" s="70"/>
       <c r="E58" s="40"/>
       <c r="F58" s="46"/>
       <c r="G58" s="45"/>
@@ -6768,11 +6768,11 @@
       <c r="B59" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C59" s="76">
+      <c r="C59" s="70">
         <f>C58-C61-C62</f>
         <v>285000</v>
       </c>
-      <c r="D59" s="76"/>
+      <c r="D59" s="70"/>
       <c r="E59" s="40">
         <f>C59/C57*100</f>
         <v>81.180726747773051</v>
@@ -6789,11 +6789,11 @@
       <c r="B60" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C60" s="73">
+      <c r="C60" s="67">
         <f>C57-C59</f>
         <v>66068.54966387467</v>
       </c>
-      <c r="D60" s="73"/>
+      <c r="D60" s="67"/>
       <c r="E60" s="40">
         <f>100-E59</f>
         <v>18.819273252226949</v>
@@ -6810,11 +6810,11 @@
       <c r="B61" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="73">
+      <c r="C61" s="67">
         <f>C58*0.03</f>
         <v>9000</v>
       </c>
-      <c r="D61" s="73"/>
+      <c r="D61" s="67"/>
       <c r="E61" s="40">
         <v>3</v>
       </c>
@@ -6830,11 +6830,1738 @@
       <c r="B62" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C62" s="73">
+      <c r="C62" s="67">
         <f>C58*0.02</f>
         <v>6000</v>
       </c>
-      <c r="D62" s="73"/>
+      <c r="D62" s="67"/>
+      <c r="E62" s="40">
+        <v>2</v>
+      </c>
+      <c r="F62" s="46"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="45"/>
+      <c r="I62" s="45"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="46"/>
+    </row>
+    <row r="63" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="54"/>
+      <c r="B63" s="54"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="54"/>
+      <c r="E63" s="54"/>
+      <c r="F63" s="54"/>
+      <c r="G63" s="54"/>
+      <c r="H63" s="54"/>
+      <c r="I63" s="54"/>
+      <c r="J63" s="54"/>
+      <c r="K63" s="54"/>
+    </row>
+    <row r="64" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+  </mergeCells>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:
+&amp;RApproved By:
+</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q64"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+    </row>
+    <row r="5" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
+        <v>1</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="21"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1</v>
+      </c>
+      <c r="D10" s="20">
+        <f>32/3.281</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E10" s="21">
+        <f>19/3.281</f>
+        <v>5.790917403230722</v>
+      </c>
+      <c r="F10" s="21">
+        <v>0.125</v>
+      </c>
+      <c r="G10" s="40">
+        <f>PRODUCT(C10:F10)</f>
+        <v>7.0599419728506199</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="21"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="19">
+        <v>2</v>
+      </c>
+      <c r="D11" s="20">
+        <f>32/3.281</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E11" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="G11" s="40">
+        <f t="shared" ref="G11:G13" si="0">PRODUCT(C11:F11)</f>
+        <v>1.0318805242304177</v>
+      </c>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="21"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="19">
+        <v>3</v>
+      </c>
+      <c r="D12" s="20">
+        <f>18.75/3.281</f>
+        <v>5.7147211216092648</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="G12" s="40">
+        <f t="shared" si="0"/>
+        <v>0.90692624199939043</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="21"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="19">
+        <v>2</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="E13" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="G13" s="40">
+        <f t="shared" si="0"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="21"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="23">
+        <f>SUM(G10:G13)</f>
+        <v>9.0527487390804282</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="23">
+        <v>13568.9</v>
+      </c>
+      <c r="J14" s="42">
+        <f>G14*I14</f>
+        <v>122835.84236570842</v>
+      </c>
+      <c r="K14" s="21"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="42">
+        <f>0.13*G14*9524.2</f>
+        <v>11208.624640297478</v>
+      </c>
+      <c r="K15" s="21"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="21"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
+        <v>2</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="21"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="38" t="str">
+        <f>B10</f>
+        <v>-slab</v>
+      </c>
+      <c r="C18" s="19">
+        <f>C10</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="20">
+        <f>D10</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E18" s="21">
+        <f>E10</f>
+        <v>5.790917403230722</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="40">
+        <f>PRODUCT(C18:F18)</f>
+        <v>56.479535782804959</v>
+      </c>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="21"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="B19" s="38" t="str">
+        <f>B11</f>
+        <v>-beam</v>
+      </c>
+      <c r="C19" s="19">
+        <f>C11</f>
+        <v>2</v>
+      </c>
+      <c r="D19" s="20">
+        <f>D11</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21">
+        <f>F11*2</f>
+        <v>0.46</v>
+      </c>
+      <c r="G19" s="40">
+        <f t="shared" ref="G19:G21" si="1">PRODUCT(C19:F19)</f>
+        <v>8.9728741237427609</v>
+      </c>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="21"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="19">
+        <f>C12</f>
+        <v>3</v>
+      </c>
+      <c r="D20" s="20">
+        <f>D12</f>
+        <v>5.7147211216092648</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21">
+        <f>F12*2</f>
+        <v>0.46</v>
+      </c>
+      <c r="G20" s="40">
+        <f t="shared" si="1"/>
+        <v>7.8863151478207856</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="21"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
+      <c r="B21" s="38" t="str">
+        <f>B13</f>
+        <v>-column</v>
+      </c>
+      <c r="C21" s="19">
+        <f>C13</f>
+        <v>2</v>
+      </c>
+      <c r="D21" s="20">
+        <f>D13*4</f>
+        <v>1.2</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21">
+        <f>F13</f>
+        <v>0.3</v>
+      </c>
+      <c r="G21" s="40">
+        <f t="shared" si="1"/>
+        <v>0.72</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="21"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18"/>
+      <c r="B22" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="23">
+        <f>SUM(G18:G21)</f>
+        <v>74.058725054368495</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" s="23">
+        <v>915.42</v>
+      </c>
+      <c r="J22" s="42">
+        <f>G22*I22</f>
+        <v>67794.838089270008</v>
+      </c>
+      <c r="K22" s="21"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="42">
+        <f>0.13*G22*46827.87/100</f>
+        <v>4508.4160539752247</v>
+      </c>
+      <c r="K23" s="21"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="21"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="18">
+        <v>3</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="23"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="21"/>
+    </row>
+    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18"/>
+      <c r="B26" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="19">
+        <f>5+5+7+7</f>
+        <v>24</v>
+      </c>
+      <c r="D26" s="20">
+        <f>32/3.281</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E26" s="21">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F26" s="40">
+        <f>PRODUCT(C26:E26)</f>
+        <v>92.474065043403641</v>
+      </c>
+      <c r="G26" s="64">
+        <f t="shared" ref="G26:G38" si="2">F26/1000</f>
+        <v>9.2474065043403636E-2</v>
+      </c>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="21"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="18"/>
+      <c r="B27" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="19">
+        <f>29+5+5</f>
+        <v>39</v>
+      </c>
+      <c r="D27" s="20">
+        <f>32/3.281</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E27" s="21">
+        <f t="shared" ref="E27:E36" si="3">8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F27" s="40">
+        <f t="shared" ref="F27:F38" si="4">PRODUCT(C27:E27)</f>
+        <v>150.27035569553092</v>
+      </c>
+      <c r="G27" s="64">
+        <f t="shared" si="2"/>
+        <v>0.15027035569553093</v>
+      </c>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="21"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18"/>
+      <c r="B28" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="19">
+        <f>58+5+6</f>
+        <v>69</v>
+      </c>
+      <c r="D28" s="20">
+        <f>19/3.281</f>
+        <v>5.790917403230722</v>
+      </c>
+      <c r="E28" s="21">
+        <f t="shared" si="3"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F28" s="40">
+        <f t="shared" si="4"/>
+        <v>157.85611884362262</v>
+      </c>
+      <c r="G28" s="64">
+        <f t="shared" si="2"/>
+        <v>0.15785611884362263</v>
+      </c>
+      <c r="H28" s="22"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="21"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="61">
+        <f>SUM(F26:F36)</f>
+        <v>551.40551096662023</v>
+      </c>
+      <c r="O28" s="61" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
+      <c r="B29" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="19">
+        <v>30</v>
+      </c>
+      <c r="D29" s="20">
+        <f>19/3.281</f>
+        <v>5.790917403230722</v>
+      </c>
+      <c r="E29" s="21">
+        <f t="shared" si="3"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F29" s="40">
+        <f t="shared" si="4"/>
+        <v>68.633095149401143</v>
+      </c>
+      <c r="G29" s="64">
+        <f t="shared" si="2"/>
+        <v>6.8633095149401149E-2</v>
+      </c>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="21"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
+      <c r="B30" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="19">
+        <v>15</v>
+      </c>
+      <c r="D30" s="20">
+        <f>7.083/3.281</f>
+        <v>2.1587930508991162</v>
+      </c>
+      <c r="E30" s="21">
+        <f t="shared" si="3"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F30" s="40">
+        <f t="shared" si="4"/>
+        <v>12.7928477090318</v>
+      </c>
+      <c r="G30" s="64">
+        <f t="shared" si="2"/>
+        <v>1.27928477090318E-2</v>
+      </c>
+      <c r="H30" s="22"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="21"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="19">
+        <v>15</v>
+      </c>
+      <c r="D31" s="20">
+        <f>6.5/3.281</f>
+        <v>1.9811033221578787</v>
+      </c>
+      <c r="E31" s="21">
+        <f t="shared" si="3"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F31" s="40">
+        <f t="shared" si="4"/>
+        <v>11.739871538713354</v>
+      </c>
+      <c r="G31" s="64">
+        <f t="shared" si="2"/>
+        <v>1.1739871538713354E-2</v>
+      </c>
+      <c r="H31" s="22"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="21"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="19">
+        <v>15</v>
+      </c>
+      <c r="D32" s="20">
+        <f>6.33/3.281</f>
+        <v>1.929289850655288</v>
+      </c>
+      <c r="E32" s="21">
+        <f t="shared" si="3"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F32" s="40">
+        <f t="shared" si="4"/>
+        <v>11.432828744623929</v>
+      </c>
+      <c r="G32" s="64">
+        <f t="shared" si="2"/>
+        <v>1.1432828744623929E-2</v>
+      </c>
+      <c r="H32" s="22"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="21"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="18"/>
+      <c r="B33" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="19">
+        <v>15</v>
+      </c>
+      <c r="D33" s="20">
+        <f>6.917/3.281</f>
+        <v>2.1081987199024685</v>
+      </c>
+      <c r="E33" s="21">
+        <f t="shared" si="3"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F33" s="40">
+        <f t="shared" si="4"/>
+        <v>12.493029451273888</v>
+      </c>
+      <c r="G33" s="64">
+        <f t="shared" si="2"/>
+        <v>1.2493029451273887E-2</v>
+      </c>
+      <c r="H33" s="22"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="21"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="19">
+        <v>15</v>
+      </c>
+      <c r="D34" s="20">
+        <f>6.083/3.281</f>
+        <v>1.8540079244132885</v>
+      </c>
+      <c r="E34" s="21">
+        <f t="shared" si="3"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F34" s="40">
+        <f t="shared" si="4"/>
+        <v>10.98671362615282</v>
+      </c>
+      <c r="G34" s="64">
+        <f t="shared" si="2"/>
+        <v>1.0986713626152821E-2</v>
+      </c>
+      <c r="H34" s="22"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="21"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="18"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="19">
+        <v>15</v>
+      </c>
+      <c r="D35" s="20">
+        <f>6.083/3.281</f>
+        <v>1.8540079244132885</v>
+      </c>
+      <c r="E35" s="21">
+        <f t="shared" si="3"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F35" s="40">
+        <f t="shared" si="4"/>
+        <v>10.98671362615282</v>
+      </c>
+      <c r="G35" s="64">
+        <f t="shared" si="2"/>
+        <v>1.0986713626152821E-2</v>
+      </c>
+      <c r="H35" s="22"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="21"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="19">
+        <v>15</v>
+      </c>
+      <c r="D36" s="20">
+        <f>6.5/3.281</f>
+        <v>1.9811033221578787</v>
+      </c>
+      <c r="E36" s="21">
+        <f t="shared" si="3"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F36" s="40">
+        <f t="shared" si="4"/>
+        <v>11.739871538713354</v>
+      </c>
+      <c r="G36" s="64">
+        <f t="shared" si="2"/>
+        <v>1.1739871538713354E-2</v>
+      </c>
+      <c r="H36" s="22"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="21"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="18"/>
+      <c r="B37" s="38" t="str">
+        <f>B19</f>
+        <v>-beam</v>
+      </c>
+      <c r="C37" s="19">
+        <f>2*5</f>
+        <v>10</v>
+      </c>
+      <c r="D37" s="20">
+        <f>D10</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E37" s="21">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F37" s="40">
+        <f t="shared" si="4"/>
+        <v>86.69443597819091</v>
+      </c>
+      <c r="G37" s="64">
+        <f t="shared" si="2"/>
+        <v>8.6694435978190904E-2</v>
+      </c>
+      <c r="H37" s="22"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="21"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="61" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O37" s="61">
+        <f>F39+F40</f>
+        <v>99.566031133236237</v>
+      </c>
+      <c r="P37" s="61">
+        <f>F48+F49</f>
+        <v>8.6281481481481475</v>
+      </c>
+      <c r="Q37" s="62" t="e">
+        <f>SUM(N37:P37)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="18"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="19">
+        <f>3*4</f>
+        <v>12</v>
+      </c>
+      <c r="D38" s="20">
+        <f>E10</f>
+        <v>5.790917403230722</v>
+      </c>
+      <c r="E38" s="21">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F38" s="40">
+        <f t="shared" si="4"/>
+        <v>61.76978563446103</v>
+      </c>
+      <c r="G38" s="64">
+        <f t="shared" si="2"/>
+        <v>6.1769785634461033E-2</v>
+      </c>
+      <c r="H38" s="22"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="21"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="61" t="e">
+        <f>SUM(F37+F38+F41+F42+#REF!+F47)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+    </row>
+    <row r="39" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="18"/>
+      <c r="B39" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="19">
+        <f>60*2</f>
+        <v>120</v>
+      </c>
+      <c r="D39" s="20">
+        <f>(0.3*2+(0.583/3.281)*2+0.075*2)</f>
+        <v>1.1053794574824747</v>
+      </c>
+      <c r="E39" s="21">
+        <f t="shared" ref="E39:E49" si="5">8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F39" s="40">
+        <f>PRODUCT(C39:E39)</f>
+        <v>52.403174280650653</v>
+      </c>
+      <c r="G39" s="64">
+        <f>F39/1000</f>
+        <v>5.2403174280650652E-2</v>
+      </c>
+      <c r="H39" s="22"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="21"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+    </row>
+    <row r="40" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="18"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="19">
+        <f>36*3</f>
+        <v>108</v>
+      </c>
+      <c r="D40" s="20">
+        <f>(0.3*2+(0.583/3.281)*2+0.075*2)</f>
+        <v>1.1053794574824747</v>
+      </c>
+      <c r="E40" s="21">
+        <f t="shared" si="5"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F40" s="40">
+        <f>PRODUCT(C40:E40)</f>
+        <v>47.162856852585584</v>
+      </c>
+      <c r="G40" s="64">
+        <f>F40/1000</f>
+        <v>4.7162856852585582E-2</v>
+      </c>
+      <c r="H40" s="22"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="21"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="19">
+        <v>6</v>
+      </c>
+      <c r="D41" s="20">
+        <f>7.75/3.281</f>
+        <v>2.3620847302651629</v>
+      </c>
+      <c r="E41" s="21">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F41" s="40">
+        <f t="shared" ref="F41:F47" si="6">PRODUCT(C41:E41)</f>
+        <v>12.597785228080866</v>
+      </c>
+      <c r="G41" s="64">
+        <f t="shared" ref="G41:G49" si="7">F41/1000</f>
+        <v>1.2597785228080867E-2</v>
+      </c>
+      <c r="H41" s="22"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="21"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+    </row>
+    <row r="42" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="19">
+        <v>1</v>
+      </c>
+      <c r="D42" s="20">
+        <f>8.667/3.281</f>
+        <v>2.6415726912526667</v>
+      </c>
+      <c r="E42" s="21">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F42" s="40">
+        <f t="shared" si="6"/>
+        <v>2.3480646144468147</v>
+      </c>
+      <c r="G42" s="64">
+        <f t="shared" si="7"/>
+        <v>2.3480646144468146E-3</v>
+      </c>
+      <c r="H42" s="22"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="21"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+    </row>
+    <row r="43" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="18"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="19">
+        <v>1</v>
+      </c>
+      <c r="D43" s="20">
+        <f>D38</f>
+        <v>5.790917403230722</v>
+      </c>
+      <c r="E43" s="21">
+        <f t="shared" ref="E43:E47" si="8">12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F43" s="40">
+        <f t="shared" si="6"/>
+        <v>5.1474821362050855</v>
+      </c>
+      <c r="G43" s="64">
+        <f t="shared" si="7"/>
+        <v>5.1474821362050855E-3</v>
+      </c>
+      <c r="H43" s="22"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="21"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+    </row>
+    <row r="44" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="18"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="19">
+        <v>1</v>
+      </c>
+      <c r="D44" s="20">
+        <f>7.667/3.281</f>
+        <v>2.3367875647668392</v>
+      </c>
+      <c r="E44" s="21">
+        <f t="shared" si="8"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F44" s="40">
+        <f t="shared" si="6"/>
+        <v>2.0771445020149679</v>
+      </c>
+      <c r="G44" s="64">
+        <f t="shared" si="7"/>
+        <v>2.0771445020149677E-3</v>
+      </c>
+      <c r="H44" s="22"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="21"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+    </row>
+    <row r="45" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="18"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="19">
+        <v>2</v>
+      </c>
+      <c r="D45" s="20">
+        <f>9/3.281</f>
+        <v>2.7430661383724475</v>
+      </c>
+      <c r="E45" s="21">
+        <f t="shared" si="8"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F45" s="40">
+        <f t="shared" si="6"/>
+        <v>4.8765620237732401</v>
+      </c>
+      <c r="G45" s="64">
+        <f t="shared" si="7"/>
+        <v>4.8765620237732404E-3</v>
+      </c>
+      <c r="H45" s="22"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="21"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+    </row>
+    <row r="46" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="18"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="19">
+        <v>2</v>
+      </c>
+      <c r="D46" s="20">
+        <f>9/3.281</f>
+        <v>2.7430661383724475</v>
+      </c>
+      <c r="E46" s="21">
+        <f t="shared" si="8"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F46" s="40">
+        <f t="shared" si="6"/>
+        <v>4.8765620237732401</v>
+      </c>
+      <c r="G46" s="64">
+        <f t="shared" si="7"/>
+        <v>4.8765620237732404E-3</v>
+      </c>
+      <c r="H46" s="22"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="21"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+    </row>
+    <row r="47" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="18"/>
+      <c r="B47" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="19">
+        <f>6*8</f>
+        <v>48</v>
+      </c>
+      <c r="D47" s="20">
+        <f>11.5/3.281</f>
+        <v>3.5050289545870159</v>
+      </c>
+      <c r="E47" s="21">
+        <f t="shared" si="8"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F47" s="40">
+        <f t="shared" si="6"/>
+        <v>149.54790206237934</v>
+      </c>
+      <c r="G47" s="64">
+        <f t="shared" si="7"/>
+        <v>0.14954790206237933</v>
+      </c>
+      <c r="H47" s="22"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="42"/>
+      <c r="K47" s="21"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+    </row>
+    <row r="48" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="18"/>
+      <c r="B48" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="19">
+        <f>(TRUNC(((8.917/3.281)/0.125),0)+1)*0+12</f>
+        <v>12</v>
+      </c>
+      <c r="D48" s="20">
+        <f>(0.23*4+0.075*2)</f>
+        <v>1.07</v>
+      </c>
+      <c r="E48" s="21">
+        <f t="shared" si="5"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F48" s="40">
+        <f>PRODUCT(C48:E48)</f>
+        <v>5.0725925925925921</v>
+      </c>
+      <c r="G48" s="64">
+        <f t="shared" si="7"/>
+        <v>5.0725925925925921E-3</v>
+      </c>
+      <c r="H48" s="22"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="21"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+    </row>
+    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="18"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="19">
+        <f>(TRUNC(((8.917/3.281)/0.125),0)+1)*0+12</f>
+        <v>12</v>
+      </c>
+      <c r="D49" s="20">
+        <f>(0.15*4+0.075*2)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E49" s="21">
+        <f t="shared" si="5"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F49" s="40">
+        <f>PRODUCT(C49:E49)</f>
+        <v>3.5555555555555554</v>
+      </c>
+      <c r="G49" s="64">
+        <f t="shared" si="7"/>
+        <v>3.5555555555555553E-3</v>
+      </c>
+      <c r="H49" s="22"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="42"/>
+      <c r="K49" s="21"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+    </row>
+    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="18"/>
+      <c r="B50" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="19"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="65">
+        <f>SUM(G26:G49)</f>
+        <v>0.9895354144513302</v>
+      </c>
+      <c r="H50" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I50" s="23">
+        <v>131940</v>
+      </c>
+      <c r="J50" s="42">
+        <f>G50*I50</f>
+        <v>130559.30258270851</v>
+      </c>
+      <c r="K50" s="21"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+    </row>
+    <row r="51" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="18"/>
+      <c r="B51" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="42">
+        <f>0.13*G50*106200</f>
+        <v>13661.525931915065</v>
+      </c>
+      <c r="K51" s="21"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+    </row>
+    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="18"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="42"/>
+      <c r="K52" s="21"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+    </row>
+    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="18">
+        <v>4</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" s="19">
+        <v>1</v>
+      </c>
+      <c r="D53" s="20"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="33">
+        <f t="shared" ref="G53" si="9">PRODUCT(C53:F53)</f>
+        <v>1</v>
+      </c>
+      <c r="H53" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I53" s="23">
+        <v>500</v>
+      </c>
+      <c r="J53" s="33">
+        <f>G53*I53</f>
+        <v>500</v>
+      </c>
+      <c r="K53" s="21"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+    </row>
+    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="18"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="42"/>
+      <c r="K54" s="21"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55" s="41"/>
+      <c r="B55" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="44"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="42"/>
+      <c r="I55" s="42"/>
+      <c r="J55" s="42">
+        <f>SUM(J9:J53)</f>
+        <v>351068.54966387467</v>
+      </c>
+      <c r="K55" s="37"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56" s="55"/>
+      <c r="B56" s="58"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="57"/>
+      <c r="H56" s="57"/>
+      <c r="I56" s="57"/>
+      <c r="J56" s="57"/>
+      <c r="K56" s="54"/>
+    </row>
+    <row r="57" spans="1:16" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="47"/>
+      <c r="B57" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="67">
+        <f>J55</f>
+        <v>351068.54966387467</v>
+      </c>
+      <c r="D57" s="67"/>
+      <c r="E57" s="40">
+        <v>100</v>
+      </c>
+      <c r="F57" s="48"/>
+      <c r="G57" s="49"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="50"/>
+      <c r="J57" s="51"/>
+      <c r="K57" s="52"/>
+    </row>
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="53"/>
+      <c r="B58" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="70">
+        <v>300000</v>
+      </c>
+      <c r="D58" s="70"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="46"/>
+    </row>
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="53"/>
+      <c r="B59" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="70">
+        <f>C58-C61-C62</f>
+        <v>285000</v>
+      </c>
+      <c r="D59" s="70"/>
+      <c r="E59" s="40">
+        <f>C59/C57*100</f>
+        <v>81.180726747773051</v>
+      </c>
+      <c r="F59" s="46"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="45"/>
+      <c r="K59" s="46"/>
+    </row>
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="53"/>
+      <c r="B60" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="67">
+        <f>C57-C59</f>
+        <v>66068.54966387467</v>
+      </c>
+      <c r="D60" s="67"/>
+      <c r="E60" s="40">
+        <f>100-E59</f>
+        <v>18.819273252226949</v>
+      </c>
+      <c r="F60" s="46"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="45"/>
+      <c r="J60" s="45"/>
+      <c r="K60" s="46"/>
+    </row>
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="53"/>
+      <c r="B61" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="67">
+        <f>C58*0.03</f>
+        <v>9000</v>
+      </c>
+      <c r="D61" s="67"/>
+      <c r="E61" s="40">
+        <v>3</v>
+      </c>
+      <c r="F61" s="46"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="45"/>
+      <c r="I61" s="45"/>
+      <c r="J61" s="45"/>
+      <c r="K61" s="46"/>
+    </row>
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="53"/>
+      <c r="B62" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" s="67">
+        <f>C58*0.02</f>
+        <v>6000</v>
+      </c>
+      <c r="D62" s="67"/>
       <c r="E62" s="40">
         <v>2</v>
       </c>
@@ -6877,1740 +8604,13 @@
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;LPrepared By:
-Kristal Suwal&amp;CChecked By:
-Er. Milan Phuyal&amp;RApproved By:
-Er. Prakash Singh Saud</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q64"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-    </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-    </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-    </row>
-    <row r="5" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-    </row>
-    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-    </row>
-    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="75" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="18">
-        <v>1</v>
-      </c>
-      <c r="B9" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="21"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="19">
-        <v>1</v>
-      </c>
-      <c r="D10" s="20">
-        <f>32/3.281</f>
-        <v>9.7531240475464784</v>
-      </c>
-      <c r="E10" s="21">
-        <f>19/3.281</f>
-        <v>5.790917403230722</v>
-      </c>
-      <c r="F10" s="21">
-        <v>0.125</v>
-      </c>
-      <c r="G10" s="40">
-        <f>PRODUCT(C10:F10)</f>
-        <v>7.0599419728506199</v>
-      </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="21"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="19">
-        <v>2</v>
-      </c>
-      <c r="D11" s="20">
-        <f>32/3.281</f>
-        <v>9.7531240475464784</v>
-      </c>
-      <c r="E11" s="21">
-        <v>0.23</v>
-      </c>
-      <c r="F11" s="21">
-        <v>0.23</v>
-      </c>
-      <c r="G11" s="40">
-        <f t="shared" ref="G11:G13" si="0">PRODUCT(C11:F11)</f>
-        <v>1.0318805242304177</v>
-      </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="21"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="19">
-        <v>3</v>
-      </c>
-      <c r="D12" s="20">
-        <f>18.75/3.281</f>
-        <v>5.7147211216092648</v>
-      </c>
-      <c r="E12" s="21">
-        <v>0.23</v>
-      </c>
-      <c r="F12" s="21">
-        <v>0.23</v>
-      </c>
-      <c r="G12" s="40">
-        <f t="shared" si="0"/>
-        <v>0.90692624199939043</v>
-      </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="21"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="19">
-        <v>2</v>
-      </c>
-      <c r="D13" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="E13" s="21">
-        <v>0.3</v>
-      </c>
-      <c r="F13" s="21">
-        <v>0.3</v>
-      </c>
-      <c r="G13" s="40">
-        <f t="shared" si="0"/>
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="21"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="23">
-        <f>SUM(G10:G13)</f>
-        <v>9.0527487390804282</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" s="23">
-        <v>13568.9</v>
-      </c>
-      <c r="J14" s="42">
-        <f>G14*I14</f>
-        <v>122835.84236570842</v>
-      </c>
-      <c r="K14" s="21"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="42">
-        <f>0.13*G14*9524.2</f>
-        <v>11208.624640297478</v>
-      </c>
-      <c r="K15" s="21"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="21"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="1:16" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
-        <v>2</v>
-      </c>
-      <c r="B17" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="21"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-    </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="38" t="str">
-        <f>B10</f>
-        <v>-slab</v>
-      </c>
-      <c r="C18" s="19">
-        <f>C10</f>
-        <v>1</v>
-      </c>
-      <c r="D18" s="20">
-        <f>D10</f>
-        <v>9.7531240475464784</v>
-      </c>
-      <c r="E18" s="21">
-        <f>E10</f>
-        <v>5.790917403230722</v>
-      </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="40">
-        <f>PRODUCT(C18:F18)</f>
-        <v>56.479535782804959</v>
-      </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="21"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-    </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="38" t="str">
-        <f>B11</f>
-        <v>-beam</v>
-      </c>
-      <c r="C19" s="19">
-        <f>C11</f>
-        <v>2</v>
-      </c>
-      <c r="D19" s="20">
-        <f>D11</f>
-        <v>9.7531240475464784</v>
-      </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21">
-        <f>F11*2</f>
-        <v>0.46</v>
-      </c>
-      <c r="G19" s="40">
-        <f t="shared" ref="G19:G21" si="1">PRODUCT(C19:F19)</f>
-        <v>8.9728741237427609</v>
-      </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="21"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="19">
-        <f>C12</f>
-        <v>3</v>
-      </c>
-      <c r="D20" s="20">
-        <f>D12</f>
-        <v>5.7147211216092648</v>
-      </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21">
-        <f>F12*2</f>
-        <v>0.46</v>
-      </c>
-      <c r="G20" s="40">
-        <f t="shared" si="1"/>
-        <v>7.8863151478207856</v>
-      </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="21"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-    </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="38" t="str">
-        <f>B13</f>
-        <v>-column</v>
-      </c>
-      <c r="C21" s="19">
-        <f>C13</f>
-        <v>2</v>
-      </c>
-      <c r="D21" s="20">
-        <f>D13*4</f>
-        <v>1.2</v>
-      </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21">
-        <f>F13</f>
-        <v>0.3</v>
-      </c>
-      <c r="G21" s="40">
-        <f t="shared" si="1"/>
-        <v>0.72</v>
-      </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="21"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-    </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="23">
-        <f>SUM(G18:G21)</f>
-        <v>74.058725054368495</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="I22" s="23">
-        <v>915.42</v>
-      </c>
-      <c r="J22" s="42">
-        <f>G22*I22</f>
-        <v>67794.838089270008</v>
-      </c>
-      <c r="K22" s="21"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-    </row>
-    <row r="23" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="42">
-        <f>0.13*G22*46827.87/100</f>
-        <v>4508.4160539752247</v>
-      </c>
-      <c r="K23" s="21"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-    </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="21"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-    </row>
-    <row r="25" spans="1:16" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="18">
-        <v>3</v>
-      </c>
-      <c r="B25" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="23"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="21"/>
-    </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="19">
-        <f>5+5+7+7</f>
-        <v>24</v>
-      </c>
-      <c r="D26" s="20">
-        <f>32/3.281</f>
-        <v>9.7531240475464784</v>
-      </c>
-      <c r="E26" s="21">
-        <f>8*8/162</f>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F26" s="40">
-        <f>PRODUCT(C26:E26)</f>
-        <v>92.474065043403641</v>
-      </c>
-      <c r="G26" s="64">
-        <f t="shared" ref="G26:G38" si="2">F26/1000</f>
-        <v>9.2474065043403636E-2</v>
-      </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="21"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-    </row>
-    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="19">
-        <f>29+5+5</f>
-        <v>39</v>
-      </c>
-      <c r="D27" s="20">
-        <f>32/3.281</f>
-        <v>9.7531240475464784</v>
-      </c>
-      <c r="E27" s="21">
-        <f t="shared" ref="E27:E36" si="3">8*8/162</f>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F27" s="40">
-        <f t="shared" ref="F27:F38" si="4">PRODUCT(C27:E27)</f>
-        <v>150.27035569553092</v>
-      </c>
-      <c r="G27" s="64">
-        <f t="shared" si="2"/>
-        <v>0.15027035569553093</v>
-      </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="21"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-    </row>
-    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
-      <c r="B28" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="19">
-        <f>58+5+6</f>
-        <v>69</v>
-      </c>
-      <c r="D28" s="20">
-        <f>19/3.281</f>
-        <v>5.790917403230722</v>
-      </c>
-      <c r="E28" s="21">
-        <f t="shared" si="3"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F28" s="40">
-        <f t="shared" si="4"/>
-        <v>157.85611884362262</v>
-      </c>
-      <c r="G28" s="64">
-        <f t="shared" si="2"/>
-        <v>0.15785611884362263</v>
-      </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="21"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="61">
-        <f>SUM(F26:F36)</f>
-        <v>551.40551096662023</v>
-      </c>
-      <c r="O28" s="61" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P28" s="1"/>
-    </row>
-    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
-      <c r="B29" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="19">
-        <v>30</v>
-      </c>
-      <c r="D29" s="20">
-        <f>19/3.281</f>
-        <v>5.790917403230722</v>
-      </c>
-      <c r="E29" s="21">
-        <f t="shared" si="3"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F29" s="40">
-        <f t="shared" si="4"/>
-        <v>68.633095149401143</v>
-      </c>
-      <c r="G29" s="64">
-        <f t="shared" si="2"/>
-        <v>6.8633095149401149E-2</v>
-      </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="21"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-    </row>
-    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
-      <c r="B30" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="19">
-        <v>15</v>
-      </c>
-      <c r="D30" s="20">
-        <f>7.083/3.281</f>
-        <v>2.1587930508991162</v>
-      </c>
-      <c r="E30" s="21">
-        <f t="shared" si="3"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F30" s="40">
-        <f t="shared" si="4"/>
-        <v>12.7928477090318</v>
-      </c>
-      <c r="G30" s="64">
-        <f t="shared" si="2"/>
-        <v>1.27928477090318E-2</v>
-      </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="21"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-    </row>
-    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="19">
-        <v>15</v>
-      </c>
-      <c r="D31" s="20">
-        <f>6.5/3.281</f>
-        <v>1.9811033221578787</v>
-      </c>
-      <c r="E31" s="21">
-        <f t="shared" si="3"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F31" s="40">
-        <f t="shared" si="4"/>
-        <v>11.739871538713354</v>
-      </c>
-      <c r="G31" s="64">
-        <f t="shared" si="2"/>
-        <v>1.1739871538713354E-2</v>
-      </c>
-      <c r="H31" s="22"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="21"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-    </row>
-    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="19">
-        <v>15</v>
-      </c>
-      <c r="D32" s="20">
-        <f>6.33/3.281</f>
-        <v>1.929289850655288</v>
-      </c>
-      <c r="E32" s="21">
-        <f t="shared" si="3"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F32" s="40">
-        <f t="shared" si="4"/>
-        <v>11.432828744623929</v>
-      </c>
-      <c r="G32" s="64">
-        <f t="shared" si="2"/>
-        <v>1.1432828744623929E-2</v>
-      </c>
-      <c r="H32" s="22"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="21"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-    </row>
-    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="19">
-        <v>15</v>
-      </c>
-      <c r="D33" s="20">
-        <f>6.917/3.281</f>
-        <v>2.1081987199024685</v>
-      </c>
-      <c r="E33" s="21">
-        <f t="shared" si="3"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F33" s="40">
-        <f t="shared" si="4"/>
-        <v>12.493029451273888</v>
-      </c>
-      <c r="G33" s="64">
-        <f t="shared" si="2"/>
-        <v>1.2493029451273887E-2</v>
-      </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="21"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-    </row>
-    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="19">
-        <v>15</v>
-      </c>
-      <c r="D34" s="20">
-        <f>6.083/3.281</f>
-        <v>1.8540079244132885</v>
-      </c>
-      <c r="E34" s="21">
-        <f t="shared" si="3"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F34" s="40">
-        <f t="shared" si="4"/>
-        <v>10.98671362615282</v>
-      </c>
-      <c r="G34" s="64">
-        <f t="shared" si="2"/>
-        <v>1.0986713626152821E-2</v>
-      </c>
-      <c r="H34" s="22"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="21"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-    </row>
-    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="19">
-        <v>15</v>
-      </c>
-      <c r="D35" s="20">
-        <f>6.083/3.281</f>
-        <v>1.8540079244132885</v>
-      </c>
-      <c r="E35" s="21">
-        <f t="shared" si="3"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F35" s="40">
-        <f t="shared" si="4"/>
-        <v>10.98671362615282</v>
-      </c>
-      <c r="G35" s="64">
-        <f t="shared" si="2"/>
-        <v>1.0986713626152821E-2</v>
-      </c>
-      <c r="H35" s="22"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="21"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-    </row>
-    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="19">
-        <v>15</v>
-      </c>
-      <c r="D36" s="20">
-        <f>6.5/3.281</f>
-        <v>1.9811033221578787</v>
-      </c>
-      <c r="E36" s="21">
-        <f t="shared" si="3"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F36" s="40">
-        <f t="shared" si="4"/>
-        <v>11.739871538713354</v>
-      </c>
-      <c r="G36" s="64">
-        <f t="shared" si="2"/>
-        <v>1.1739871538713354E-2</v>
-      </c>
-      <c r="H36" s="22"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="21"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-    </row>
-    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="18"/>
-      <c r="B37" s="38" t="str">
-        <f>B19</f>
-        <v>-beam</v>
-      </c>
-      <c r="C37" s="19">
-        <f>2*5</f>
-        <v>10</v>
-      </c>
-      <c r="D37" s="20">
-        <f>D10</f>
-        <v>9.7531240475464784</v>
-      </c>
-      <c r="E37" s="21">
-        <f>12*12/162</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F37" s="40">
-        <f t="shared" si="4"/>
-        <v>86.69443597819091</v>
-      </c>
-      <c r="G37" s="64">
-        <f t="shared" si="2"/>
-        <v>8.6694435978190904E-2</v>
-      </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="42"/>
-      <c r="K37" s="21"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="61" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O37" s="61">
-        <f>F39+F40</f>
-        <v>99.566031133236237</v>
-      </c>
-      <c r="P37" s="61">
-        <f>F48+F49</f>
-        <v>8.6281481481481475</v>
-      </c>
-      <c r="Q37" s="62" t="e">
-        <f>SUM(N37:P37)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="19">
-        <f>3*4</f>
-        <v>12</v>
-      </c>
-      <c r="D38" s="20">
-        <f>E10</f>
-        <v>5.790917403230722</v>
-      </c>
-      <c r="E38" s="21">
-        <f>12*12/162</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F38" s="40">
-        <f t="shared" si="4"/>
-        <v>61.76978563446103</v>
-      </c>
-      <c r="G38" s="64">
-        <f t="shared" si="2"/>
-        <v>6.1769785634461033E-2</v>
-      </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="21"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="61" t="e">
-        <f>SUM(F37+F38+F41+F42+#REF!+F47)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-    </row>
-    <row r="39" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="18"/>
-      <c r="B39" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="19">
-        <f>60*2</f>
-        <v>120</v>
-      </c>
-      <c r="D39" s="20">
-        <f>(0.3*2+(0.583/3.281)*2+0.075*2)</f>
-        <v>1.1053794574824747</v>
-      </c>
-      <c r="E39" s="21">
-        <f t="shared" ref="E39:E49" si="5">8*8/162</f>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F39" s="40">
-        <f>PRODUCT(C39:E39)</f>
-        <v>52.403174280650653</v>
-      </c>
-      <c r="G39" s="64">
-        <f>F39/1000</f>
-        <v>5.2403174280650652E-2</v>
-      </c>
-      <c r="H39" s="22"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="42"/>
-      <c r="K39" s="21"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-    </row>
-    <row r="40" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="18"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="19">
-        <f>36*3</f>
-        <v>108</v>
-      </c>
-      <c r="D40" s="20">
-        <f>(0.3*2+(0.583/3.281)*2+0.075*2)</f>
-        <v>1.1053794574824747</v>
-      </c>
-      <c r="E40" s="21">
-        <f t="shared" si="5"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F40" s="40">
-        <f>PRODUCT(C40:E40)</f>
-        <v>47.162856852585584</v>
-      </c>
-      <c r="G40" s="64">
-        <f>F40/1000</f>
-        <v>4.7162856852585582E-2</v>
-      </c>
-      <c r="H40" s="22"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="42"/>
-      <c r="K40" s="21"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-    </row>
-    <row r="41" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18"/>
-      <c r="B41" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="19">
-        <v>6</v>
-      </c>
-      <c r="D41" s="20">
-        <f>7.75/3.281</f>
-        <v>2.3620847302651629</v>
-      </c>
-      <c r="E41" s="21">
-        <f>12*12/162</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F41" s="40">
-        <f t="shared" ref="F41:F47" si="6">PRODUCT(C41:E41)</f>
-        <v>12.597785228080866</v>
-      </c>
-      <c r="G41" s="64">
-        <f t="shared" ref="G41:G49" si="7">F41/1000</f>
-        <v>1.2597785228080867E-2</v>
-      </c>
-      <c r="H41" s="22"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="42"/>
-      <c r="K41" s="21"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-    </row>
-    <row r="42" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="18"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="19">
-        <v>1</v>
-      </c>
-      <c r="D42" s="20">
-        <f>8.667/3.281</f>
-        <v>2.6415726912526667</v>
-      </c>
-      <c r="E42" s="21">
-        <f>12*12/162</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F42" s="40">
-        <f t="shared" si="6"/>
-        <v>2.3480646144468147</v>
-      </c>
-      <c r="G42" s="64">
-        <f t="shared" si="7"/>
-        <v>2.3480646144468146E-3</v>
-      </c>
-      <c r="H42" s="22"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="21"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-    </row>
-    <row r="43" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="18"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="19">
-        <v>1</v>
-      </c>
-      <c r="D43" s="20">
-        <f>D38</f>
-        <v>5.790917403230722</v>
-      </c>
-      <c r="E43" s="21">
-        <f t="shared" ref="E43:E47" si="8">12*12/162</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F43" s="40">
-        <f t="shared" si="6"/>
-        <v>5.1474821362050855</v>
-      </c>
-      <c r="G43" s="64">
-        <f t="shared" si="7"/>
-        <v>5.1474821362050855E-3</v>
-      </c>
-      <c r="H43" s="22"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="21"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-    </row>
-    <row r="44" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="18"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="19">
-        <v>1</v>
-      </c>
-      <c r="D44" s="20">
-        <f>7.667/3.281</f>
-        <v>2.3367875647668392</v>
-      </c>
-      <c r="E44" s="21">
-        <f t="shared" si="8"/>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F44" s="40">
-        <f t="shared" si="6"/>
-        <v>2.0771445020149679</v>
-      </c>
-      <c r="G44" s="64">
-        <f t="shared" si="7"/>
-        <v>2.0771445020149677E-3</v>
-      </c>
-      <c r="H44" s="22"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="42"/>
-      <c r="K44" s="21"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-    </row>
-    <row r="45" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="19">
-        <v>2</v>
-      </c>
-      <c r="D45" s="20">
-        <f>9/3.281</f>
-        <v>2.7430661383724475</v>
-      </c>
-      <c r="E45" s="21">
-        <f t="shared" si="8"/>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F45" s="40">
-        <f t="shared" si="6"/>
-        <v>4.8765620237732401</v>
-      </c>
-      <c r="G45" s="64">
-        <f t="shared" si="7"/>
-        <v>4.8765620237732404E-3</v>
-      </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="42"/>
-      <c r="K45" s="21"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-    </row>
-    <row r="46" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="18"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="19">
-        <v>2</v>
-      </c>
-      <c r="D46" s="20">
-        <f>9/3.281</f>
-        <v>2.7430661383724475</v>
-      </c>
-      <c r="E46" s="21">
-        <f t="shared" si="8"/>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F46" s="40">
-        <f t="shared" si="6"/>
-        <v>4.8765620237732401</v>
-      </c>
-      <c r="G46" s="64">
-        <f t="shared" si="7"/>
-        <v>4.8765620237732404E-3</v>
-      </c>
-      <c r="H46" s="22"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="21"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-    </row>
-    <row r="47" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="18"/>
-      <c r="B47" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="19">
-        <f>6*8</f>
-        <v>48</v>
-      </c>
-      <c r="D47" s="20">
-        <f>11.5/3.281</f>
-        <v>3.5050289545870159</v>
-      </c>
-      <c r="E47" s="21">
-        <f t="shared" si="8"/>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F47" s="40">
-        <f t="shared" si="6"/>
-        <v>149.54790206237934</v>
-      </c>
-      <c r="G47" s="64">
-        <f t="shared" si="7"/>
-        <v>0.14954790206237933</v>
-      </c>
-      <c r="H47" s="22"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="42"/>
-      <c r="K47" s="21"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-    </row>
-    <row r="48" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="18"/>
-      <c r="B48" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="19">
-        <f>(TRUNC(((8.917/3.281)/0.125),0)+1)*0+12</f>
-        <v>12</v>
-      </c>
-      <c r="D48" s="20">
-        <f>(0.23*4+0.075*2)</f>
-        <v>1.07</v>
-      </c>
-      <c r="E48" s="21">
-        <f t="shared" si="5"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F48" s="40">
-        <f>PRODUCT(C48:E48)</f>
-        <v>5.0725925925925921</v>
-      </c>
-      <c r="G48" s="64">
-        <f t="shared" si="7"/>
-        <v>5.0725925925925921E-3</v>
-      </c>
-      <c r="H48" s="22"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="21"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-    </row>
-    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="18"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="19">
-        <f>(TRUNC(((8.917/3.281)/0.125),0)+1)*0+12</f>
-        <v>12</v>
-      </c>
-      <c r="D49" s="20">
-        <f>(0.15*4+0.075*2)</f>
-        <v>0.75</v>
-      </c>
-      <c r="E49" s="21">
-        <f t="shared" si="5"/>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F49" s="40">
-        <f>PRODUCT(C49:E49)</f>
-        <v>3.5555555555555554</v>
-      </c>
-      <c r="G49" s="64">
-        <f t="shared" si="7"/>
-        <v>3.5555555555555553E-3</v>
-      </c>
-      <c r="H49" s="22"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="42"/>
-      <c r="K49" s="21"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-    </row>
-    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
-      <c r="B50" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="65">
-        <f>SUM(G26:G49)</f>
-        <v>0.9895354144513302</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="I50" s="23">
-        <v>131940</v>
-      </c>
-      <c r="J50" s="42">
-        <f>G50*I50</f>
-        <v>130559.30258270851</v>
-      </c>
-      <c r="K50" s="21"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-    </row>
-    <row r="51" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="18"/>
-      <c r="B51" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="23"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="23"/>
-      <c r="J51" s="42">
-        <f>0.13*G50*106200</f>
-        <v>13661.525931915065</v>
-      </c>
-      <c r="K51" s="21"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-    </row>
-    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="18"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="23"/>
-      <c r="J52" s="42"/>
-      <c r="K52" s="21"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-    </row>
-    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="18">
-        <v>4</v>
-      </c>
-      <c r="B53" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C53" s="19">
-        <v>1</v>
-      </c>
-      <c r="D53" s="20"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="33">
-        <f t="shared" ref="G53" si="9">PRODUCT(C53:F53)</f>
-        <v>1</v>
-      </c>
-      <c r="H53" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I53" s="23">
-        <v>500</v>
-      </c>
-      <c r="J53" s="33">
-        <f>G53*I53</f>
-        <v>500</v>
-      </c>
-      <c r="K53" s="21"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-    </row>
-    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="42"/>
-      <c r="K54" s="21"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A55" s="41"/>
-      <c r="B55" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" s="44"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="42"/>
-      <c r="J55" s="42">
-        <f>SUM(J9:J53)</f>
-        <v>351068.54966387467</v>
-      </c>
-      <c r="K55" s="37"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A56" s="55"/>
-      <c r="B56" s="58"/>
-      <c r="C56" s="59"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="57"/>
-      <c r="H56" s="57"/>
-      <c r="I56" s="57"/>
-      <c r="J56" s="57"/>
-      <c r="K56" s="54"/>
-    </row>
-    <row r="57" spans="1:16" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="47"/>
-      <c r="B57" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="73">
-        <f>J55</f>
-        <v>351068.54966387467</v>
-      </c>
-      <c r="D57" s="73"/>
-      <c r="E57" s="40">
-        <v>100</v>
-      </c>
-      <c r="F57" s="48"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="50"/>
-      <c r="J57" s="51"/>
-      <c r="K57" s="52"/>
-    </row>
-    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="53"/>
-      <c r="B58" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="76">
-        <v>300000</v>
-      </c>
-      <c r="D58" s="76"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="46"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="45"/>
-      <c r="K58" s="46"/>
-    </row>
-    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="53"/>
-      <c r="B59" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C59" s="76">
-        <f>C58-C61-C62</f>
-        <v>285000</v>
-      </c>
-      <c r="D59" s="76"/>
-      <c r="E59" s="40">
-        <f>C59/C57*100</f>
-        <v>81.180726747773051</v>
-      </c>
-      <c r="F59" s="46"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="45"/>
-      <c r="J59" s="45"/>
-      <c r="K59" s="46"/>
-    </row>
-    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="53"/>
-      <c r="B60" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C60" s="73">
-        <f>C57-C59</f>
-        <v>66068.54966387467</v>
-      </c>
-      <c r="D60" s="73"/>
-      <c r="E60" s="40">
-        <f>100-E59</f>
-        <v>18.819273252226949</v>
-      </c>
-      <c r="F60" s="46"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45"/>
-      <c r="I60" s="45"/>
-      <c r="J60" s="45"/>
-      <c r="K60" s="46"/>
-    </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="53"/>
-      <c r="B61" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C61" s="73">
-        <f>C58*0.03</f>
-        <v>9000</v>
-      </c>
-      <c r="D61" s="73"/>
-      <c r="E61" s="40">
-        <v>3</v>
-      </c>
-      <c r="F61" s="46"/>
-      <c r="G61" s="45"/>
-      <c r="H61" s="45"/>
-      <c r="I61" s="45"/>
-      <c r="J61" s="45"/>
-      <c r="K61" s="46"/>
-    </row>
-    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="53"/>
-      <c r="B62" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" s="73">
-        <f>C58*0.02</f>
-        <v>6000</v>
-      </c>
-      <c r="D62" s="73"/>
-      <c r="E62" s="40">
-        <v>2</v>
-      </c>
-      <c r="F62" s="46"/>
-      <c r="G62" s="45"/>
-      <c r="H62" s="45"/>
-      <c r="I62" s="45"/>
-      <c r="J62" s="45"/>
-      <c r="K62" s="46"/>
-    </row>
-    <row r="63" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="54"/>
-      <c r="B63" s="54"/>
-      <c r="C63" s="54"/>
-      <c r="D63" s="54"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="54"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="54"/>
-      <c r="J63" s="54"/>
-      <c r="K63" s="54"/>
-    </row>
-    <row r="64" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;LPrepared By:
-Kristal Suwal&amp;CChecked By:
-Er. Milan Phuyal&amp;RApproved By:
-Er. Prakash Singh Saud</oddFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:
+&amp;RApproved By:
+</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>